<commit_message>
- CHG: Removed chemical compounds template as it has been merged with trials.
- CHG: Updated image template to remove compound references.
</commit_message>
<xml_diff>
--- a/images/example-images.xlsx
+++ b/images/example-images.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sr41756\workspaces\misc\germinate-data-templates\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC42DFD-3888-451D-BAE8-4209C52457E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAF300B-7A65-48BE-B017-8D40CB22D1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{62910211-CFC4-431D-B4FC-F3CA2666BD3A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{62910211-CFC4-431D-B4FC-F3CA2666BD3A}"/>
   </bookViews>
   <sheets>
     <sheet name="METADATA" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
   <si>
     <t>Image filename</t>
   </si>
@@ -234,9 +234,6 @@
   </si>
   <si>
     <t>phenotypes</t>
-  </si>
-  <si>
-    <t>compounds</t>
   </si>
 </sst>
 </file>
@@ -376,6 +373,13 @@
     <cellStyle name="Warning Text" xfId="1" builtinId="11"/>
   </cellStyles>
   <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -476,13 +480,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -497,12 +494,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54EC72CD-72D1-4C19-9357-01954232803D}" name="Table7" displayName="Table7" ref="A1:C18" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54EC72CD-72D1-4C19-9357-01954232803D}" name="Table7" displayName="Table7" ref="A1:C18" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:C18" xr:uid="{54EC72CD-72D1-4C19-9357-01954232803D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FF0C737E-F59C-41AE-8160-6E9938524941}" name="LABEL" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{D90AD2FC-905C-4858-A478-9F597CA4F533}" name="DEFINITION" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{4F5E424B-EE57-4C7A-B33E-B57020722A53}" name="VALUE" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{FF0C737E-F59C-41AE-8160-6E9938524941}" name="LABEL" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{D90AD2FC-905C-4858-A478-9F597CA4F533}" name="DEFINITION" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{4F5E424B-EE57-4C7A-B33E-B57020722A53}" name="VALUE" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -524,8 +521,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7E740628-0F56-4658-A76D-4EFBB87C1A67}" name="Table2" displayName="Table2" ref="A1:A4" totalsRowShown="0">
-  <autoFilter ref="A1:A4" xr:uid="{7E740628-0F56-4658-A76D-4EFBB87C1A67}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7E740628-0F56-4658-A76D-4EFBB87C1A67}" name="Table2" displayName="Table2" ref="A1:A3" totalsRowShown="0">
+  <autoFilter ref="A1:A3" xr:uid="{7E740628-0F56-4658-A76D-4EFBB87C1A67}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{70982AD8-8935-4B47-8CF1-FD79E66351AA}" name="Valid types"/>
   </tableColumns>
@@ -1042,7 +1039,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C3">
-    <cfRule type="containsBlanks" dxfId="5" priority="1">
+    <cfRule type="containsBlanks" dxfId="6" priority="1">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1061,7 +1058,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,7 +1144,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:D4">
-    <cfRule type="containsBlanks" dxfId="6" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1161,7 +1158,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4FD7D685-7C5B-4649-BCD9-948BA13E5A06}">
           <x14:formula1>
-            <xm:f>TYPES!$A$2:$A$4</xm:f>
+            <xm:f>TYPES!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>C1:C1048576</xm:sqref>
         </x14:dataValidation>
@@ -1173,10 +1170,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F5D2CF-DE80-4C7A-BF4C-C232D23677A7}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,11 +1196,6 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>63</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>